<commit_message>
Subindo diagrama de solução e atualização no burndown
</commit_message>
<xml_diff>
--- a/Nike_Documentary/Backlog/BacklogNikeStepClub.xlsx
+++ b/Nike_Documentary/Backlog/BacklogNikeStepClub.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D7793CD-2C55-45B9-889F-1C5B829A7312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\OneDrive - SPTech School\Área de Trabalho\ProjetoIndividual\NikeStepClub\Nike_Documentary\Backlog\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -324,8 +328,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,6 +347,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -468,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -504,6 +516,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -703,13 +716,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -728,6 +734,13 @@
       <font>
         <color rgb="FF000000"/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -765,7 +778,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -804,6 +817,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -829,7 +843,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -919,7 +933,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7B55-48F7-A597-4EDDC6CBE710}"/>
             </c:ext>
@@ -984,19 +998,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>88</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-7B55-48F7-A597-4EDDC6CBE710}"/>
             </c:ext>
@@ -1011,11 +1025,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1992502792"/>
-        <c:axId val="1992556040"/>
+        <c:axId val="268937016"/>
+        <c:axId val="268934272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1992502792"/>
+        <c:axId val="268937016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,10 +1069,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1992556040"/>
+        <c:crossAx val="268934272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1066,7 +1080,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1992556040"/>
+        <c:axId val="268934272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,10 +1128,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1992502792"/>
+        <c:crossAx val="268937016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1131,6 +1145,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1156,7 +1171,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1186,7 +1201,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1773,7 +1788,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9EEE2FE-A99D-2EAE-B02F-FE968E9CE8D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D9EEE2FE-A99D-2EAE-B02F-FE968E9CE8D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1795,18 +1810,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{810B9907-8B31-4001-811F-CCC4D3D7476D}" name="Tabela1" displayName="Tabela1" ref="A1:I35" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:I35" xr:uid="{810B9907-8B31-4001-811F-CCC4D3D7476D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:I35" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:I35"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5C8E3FEC-1885-4A02-A4D3-51386F2B6A00}" name="Item" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{FA1B9AF3-4372-4273-BB86-E917AAE04B97}" name="Requisito" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{542987A4-AA2C-4FF7-8AE1-13513B92FE76}" name="Descrição" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{CD619164-331E-4209-888D-F37F4704C097}" name="Classificação" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{CE9F7EA1-0916-4A93-8A8A-8EFD66A8974A}" name="Tamanho" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{FEEA9E78-3922-48B2-9C74-8E97515C7DC8}" name="Tam (#)" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{37C73A54-C790-4B60-A115-9217849AC131}" name="Prioridade" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{2C119041-2ED8-4B65-AB8C-8900F4F75E33}" name="SPRINT" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{07F2DD59-432D-4E96-BFD8-1392308C4158}" name="Membro" dataDxfId="0"/>
+    <tableColumn id="1" name="Item" dataDxfId="8"/>
+    <tableColumn id="2" name="Requisito" dataDxfId="7"/>
+    <tableColumn id="3" name="Descrição" dataDxfId="6"/>
+    <tableColumn id="4" name="Classificação" dataDxfId="5"/>
+    <tableColumn id="5" name="Tamanho" dataDxfId="4"/>
+    <tableColumn id="6" name="Tam (#)" dataDxfId="3"/>
+    <tableColumn id="7" name="Prioridade" dataDxfId="2"/>
+    <tableColumn id="8" name="SPRINT" dataDxfId="1"/>
+    <tableColumn id="9" name="Membro" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2128,22 +2143,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" customWidth="1"/>
-    <col min="3" max="3" width="197.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.25" customWidth="1"/>
+    <col min="3" max="3" width="197.25" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.375" customWidth="1"/>
+    <col min="14" max="14" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -2228,11 +2243,11 @@
       </c>
       <c r="O2" s="13">
         <f>SUM(O3,O4,O5,O6,O7)</f>
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="P2" s="13">
         <f>N2-O2</f>
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -2318,11 +2333,11 @@
         <v>66</v>
       </c>
       <c r="O4" s="13">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="P4" s="13">
         <f>N4-O4</f>
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -2448,7 +2463,7 @@
       <c r="N7" s="13">
         <v>0</v>
       </c>
-      <c r="O7" s="13"/>
+      <c r="O7" s="19"/>
       <c r="P7" s="13">
         <v>0</v>
       </c>
@@ -3267,9 +3282,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Subindo atualização no burndown
</commit_message>
<xml_diff>
--- a/Nike_Documentary/Backlog/BacklogNikeStepClub.xlsx
+++ b/Nike_Documentary/Backlog/BacklogNikeStepClub.xlsx
@@ -998,13 +998,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>93</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1025,11 +1025,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="268937016"/>
-        <c:axId val="268934272"/>
+        <c:axId val="249248632"/>
+        <c:axId val="249249016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="268937016"/>
+        <c:axId val="249248632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1072,7 +1072,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="268934272"/>
+        <c:crossAx val="249249016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1080,7 +1080,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="268934272"/>
+        <c:axId val="249249016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1131,7 +1131,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="268937016"/>
+        <c:crossAx val="249248632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1788,7 +1788,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D9EEE2FE-A99D-2EAE-B02F-FE968E9CE8D2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9EEE2FE-A99D-2EAE-B02F-FE968E9CE8D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2147,7 +2147,7 @@
   <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2243,11 +2243,11 @@
       </c>
       <c r="O2" s="13">
         <f>SUM(O3,O4,O5,O6,O7)</f>
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="P2" s="13">
         <f>N2-O2</f>
-        <v>189</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -2333,11 +2333,11 @@
         <v>66</v>
       </c>
       <c r="O4" s="13">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="P4" s="13">
         <f>N4-O4</f>
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:16">

</xml_diff>

<commit_message>
Subindo atualização no gráfico de burndown
</commit_message>
<xml_diff>
--- a/Nike_Documentary/Backlog/BacklogNikeStepClub.xlsx
+++ b/Nike_Documentary/Backlog/BacklogNikeStepClub.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="97">
   <si>
     <t>Item</t>
   </si>
@@ -67,15 +67,6 @@
     <t>Pontos Fibonacci</t>
   </si>
   <si>
-    <t>Planejado</t>
-  </si>
-  <si>
-    <t>Entregue</t>
-  </si>
-  <si>
-    <t>Pendente</t>
-  </si>
-  <si>
     <t>Configurar projeto no GitHub</t>
   </si>
   <si>
@@ -145,9 +136,6 @@
     <t>Elaborar um argumento "headshot"/argumento convincente para o projeto</t>
   </si>
   <si>
-    <t>Sprint 5</t>
-  </si>
-  <si>
     <t>Desenvolver escopo do projeto</t>
   </si>
   <si>
@@ -323,6 +311,21 @@
   </si>
   <si>
     <t>Desenvolver um diagrama que torne as funcionalidades técnicas do projeto mais visíveis ao usuário</t>
+  </si>
+  <si>
+    <t>Restante</t>
+  </si>
+  <si>
+    <t>Pontos Planejados</t>
+  </si>
+  <si>
+    <t>Estimativa</t>
+  </si>
+  <si>
+    <t>Pontos Entregues</t>
+  </si>
+  <si>
+    <t>Pendentes</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,18 +384,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -476,16 +485,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -507,16 +541,31 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,9 +860,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Gráfico Burndown</a:t>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Gráfico</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> Burndown</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -854,15 +908,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$N$1</c:f>
+              <c:f>Planilha1!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Planejado</c:v>
+                  <c:v>Estimativa</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -870,20 +924,32 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Planilha1!$L$2:$L$7</c:f>
+              <c:f>Planilha1!$L$2:$L$6</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Total</c:v>
                 </c:pt>
@@ -899,56 +965,45 @@
                 <c:pt idx="4">
                   <c:v>Sprint 4</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$N$2:$N$7</c:f>
+              <c:f>Planilha1!$P$2:$P$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>282</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7B55-48F7-A597-4EDDC6CBE710}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$O$1</c:f>
+              <c:f>Planilha1!$Q$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Entregue</c:v>
+                  <c:v>Restante</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -956,20 +1011,32 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Planilha1!$L$2:$L$7</c:f>
+              <c:f>Planilha1!$L$2:$L$6</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Total</c:v>
                 </c:pt>
@@ -985,36 +1052,28 @@
                 <c:pt idx="4">
                   <c:v>Sprint 4</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$O$2:$O$7</c:f>
+              <c:f>Planilha1!$Q$2:$Q$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>106</c:v>
+                  <c:v>282</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-7B55-48F7-A597-4EDDC6CBE710}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1024,12 +1083,332 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="249248632"/>
-        <c:axId val="249249016"/>
+        <c:axId val="290317096"/>
+        <c:axId val="290314352"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$M$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Pontos Fibonacci</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$L$2:$L$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>Total</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Sprint 1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Sprint 2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Sprint 3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Sprint 4</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$M$2:$M$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>282</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>51</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>66</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>84</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>81</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$N$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Pontos Planejados</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$L$2:$L$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>Total</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Sprint 1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Sprint 2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Sprint 3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Sprint 4</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$N$2:$N$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>282</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>51</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>66</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>84</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>81</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$O$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Pontos Entregues</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$L$2:$L$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>Total</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Sprint 1</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Sprint 2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Sprint 3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Sprint 4</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Planilha1!$O$2:$O$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>114</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>51</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>63</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="249248632"/>
+        <c:axId val="290317096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1072,7 +1451,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249249016"/>
+        <c:crossAx val="290314352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1080,7 +1459,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="249249016"/>
+        <c:axId val="290314352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1131,7 +1510,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="249248632"/>
+        <c:crossAx val="290317096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1206,7 +1585,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1253,7 +1632,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1361,11 +1740,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1376,11 +1750,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1412,9 +1781,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1773,25 +2139,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9EEE2FE-A99D-2EAE-B02F-FE968E9CE8D2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2144,10 +2504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2158,11 +2518,13 @@
     <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="10.625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.375" customWidth="1"/>
-    <col min="14" max="14" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.25" customWidth="1"/>
+    <col min="16" max="16" width="10.25" customWidth="1"/>
+    <col min="18" max="18" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2186,1098 +2548,1122 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="F2" s="3">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="L2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="4">
-        <v>5</v>
-      </c>
-      <c r="G2" s="4">
-        <v>2</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="13">
+      <c r="M2" s="12">
         <f>SUM(M3,M4,M5,M6)</f>
         <v>282</v>
       </c>
-      <c r="N2" s="13">
-        <f>SUM(N3,N4,N5,N6)</f>
+      <c r="N2" s="12">
         <v>282</v>
       </c>
-      <c r="O2" s="13">
-        <f>SUM(O3,O4,O5,O6,O7)</f>
-        <v>106</v>
-      </c>
-      <c r="P2" s="13">
-        <f>N2-O2</f>
-        <v>176</v>
+      <c r="O2" s="12">
+        <f>SUM(O3,O4,O5,O6)</f>
+        <v>114</v>
+      </c>
+      <c r="P2" s="23">
+        <v>282</v>
+      </c>
+      <c r="Q2" s="22">
+        <v>282</v>
+      </c>
+      <c r="R2" s="22">
+        <f>SUM(R3,R4,R5,R6)</f>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="3">
+    <row r="3" spans="1:18">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="12">
+        <v>51</v>
+      </c>
+      <c r="N3" s="12">
+        <v>51</v>
+      </c>
+      <c r="O3" s="12">
+        <v>51</v>
+      </c>
+      <c r="P3" s="23">
+        <f>P2-N3</f>
+        <v>231</v>
+      </c>
+      <c r="Q3" s="22">
+        <f>Q2-O3</f>
+        <v>231</v>
+      </c>
+      <c r="R3" s="22">
+        <f>Q3-P3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="L4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="12">
+        <v>66</v>
+      </c>
+      <c r="N4" s="12">
+        <v>66</v>
+      </c>
+      <c r="O4" s="12">
+        <v>63</v>
+      </c>
+      <c r="P4" s="23">
+        <f>P3-N4</f>
+        <v>165</v>
+      </c>
+      <c r="Q4" s="22">
+        <f>Q3-O4</f>
+        <v>168</v>
+      </c>
+      <c r="R4" s="22">
+        <f>Q4-P4</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="4">
+      <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="17">
+        <v>84</v>
+      </c>
+      <c r="N5" s="17">
+        <v>84</v>
+      </c>
+      <c r="O5" s="17"/>
+      <c r="P5" s="16">
+        <f>P4-N5</f>
+        <v>81</v>
+      </c>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="3">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="22">
+        <v>81</v>
+      </c>
+      <c r="N6" s="22">
+        <v>81</v>
+      </c>
+      <c r="O6" s="22"/>
+      <c r="P6" s="24">
+        <f>P5-N6</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="18"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="19"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="3">
+        <v>13</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="3">
         <v>3</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="14">
+        <v>8</v>
+      </c>
+      <c r="G11" s="14">
         <v>2</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="13">
+      <c r="H11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="3">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="3">
+        <v>13</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="3">
+        <v>8</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="3">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="13">
-        <v>51</v>
-      </c>
-      <c r="O3" s="13">
-        <v>51</v>
-      </c>
-      <c r="P3" s="13">
-        <f>N3-O3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="4">
-        <v>3</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="13">
-        <v>66</v>
-      </c>
-      <c r="N4" s="13">
-        <v>66</v>
-      </c>
-      <c r="O4" s="13">
-        <v>55</v>
-      </c>
-      <c r="P4" s="13">
-        <f>N4-O4</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="3">
+        <v>21</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="4">
-        <v>8</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="13">
-        <v>84</v>
-      </c>
-      <c r="N5" s="13">
-        <v>84</v>
-      </c>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13">
-        <f>N5-O5</f>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="4">
-        <v>8</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="13">
-        <v>81</v>
-      </c>
-      <c r="N6" s="13">
-        <v>81</v>
-      </c>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13">
-        <f>N6-O6</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="4">
-        <v>8</v>
-      </c>
-      <c r="G7" s="4">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M7" s="13">
-        <v>0</v>
-      </c>
-      <c r="N7" s="13">
-        <v>0</v>
-      </c>
-      <c r="O7" s="19"/>
-      <c r="P7" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="4">
-        <v>13</v>
-      </c>
-      <c r="G8" s="4">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="4">
-        <v>3</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="4">
-        <v>3</v>
-      </c>
-      <c r="G10" s="4">
-        <v>3</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="16">
-        <v>10</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="17">
-        <v>8</v>
-      </c>
-      <c r="G11" s="17">
-        <v>2</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="4">
-        <v>8</v>
-      </c>
-      <c r="G12" s="4">
-        <v>2</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="4">
-        <v>13</v>
-      </c>
-      <c r="G13" s="4">
-        <v>2</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="4">
-        <v>8</v>
-      </c>
-      <c r="G14" s="4">
-        <v>2</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="3">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="4">
-        <v>8</v>
-      </c>
-      <c r="G15" s="4">
-        <v>2</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="3">
+      <c r="I16" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="4">
-        <v>21</v>
-      </c>
-      <c r="G16" s="4">
-        <v>2</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="B17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="3">
+        <v>8</v>
+      </c>
+      <c r="G17" s="3">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="4">
-        <v>8</v>
-      </c>
-      <c r="G17" s="4">
-        <v>2</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="4">
+      <c r="B18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="3">
         <v>5</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>2</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>18</v>
+      <c r="H18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="4">
+      <c r="B19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="3">
         <v>5</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>1</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>18</v>
+      <c r="H19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="4">
+      <c r="B20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="3">
         <v>13</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>2</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>18</v>
+      <c r="H20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="4">
+      <c r="B21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="3">
         <v>8</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>2</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>18</v>
+      <c r="H21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="4">
+      <c r="B22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="3">
         <v>8</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>2</v>
       </c>
-      <c r="H22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>18</v>
+      <c r="H22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F23" s="4">
+      <c r="B23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="3">
         <v>21</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>2</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>18</v>
+      <c r="H23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="4">
+      <c r="B24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="3">
         <v>8</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <v>2</v>
       </c>
-      <c r="H24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>18</v>
+      <c r="H24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F25" s="4">
+      <c r="B25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="3">
         <v>13</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <v>3</v>
       </c>
-      <c r="H25" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>18</v>
+      <c r="H25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="4">
+      <c r="B26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="3">
         <v>5</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <v>3</v>
       </c>
-      <c r="H26" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>18</v>
+      <c r="H26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="4">
+      <c r="B27" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="3">
         <v>8</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <v>3</v>
       </c>
-      <c r="H27" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>18</v>
+      <c r="H27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="4">
+      <c r="B28" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="3">
         <v>8</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <v>3</v>
       </c>
-      <c r="H28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>18</v>
+      <c r="H28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="3">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F29" s="4">
+      <c r="B29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="3">
         <v>8</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>3</v>
       </c>
-      <c r="H29" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>18</v>
+      <c r="H29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="4">
+      <c r="B30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="3">
         <v>5</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>3</v>
       </c>
-      <c r="H30" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>18</v>
+      <c r="H30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="6">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="7" t="s">
+      <c r="B31" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="7">
+      <c r="E31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="6">
         <v>3</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="6">
         <v>3</v>
       </c>
-      <c r="H31" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>18</v>
+      <c r="H31" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="3">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="4">
+      <c r="B32" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="3">
         <v>13</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="3">
         <v>2</v>
       </c>
-      <c r="H32" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>18</v>
+      <c r="H32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="3">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F33" s="4">
+      <c r="B33" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="3">
         <v>13</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="3">
         <v>2</v>
       </c>
-      <c r="H33" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>18</v>
+      <c r="H33" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="3">
+      <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="B34" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="3">
+        <v>5</v>
+      </c>
+      <c r="G34" s="3">
+        <v>2</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="4">
-        <v>5</v>
-      </c>
-      <c r="G34" s="4">
-        <v>2</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="6">
+      <c r="A35" s="5">
         <v>34</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="7" t="s">
+      <c r="B35" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="6">
+        <v>5</v>
+      </c>
+      <c r="G35" s="6">
+        <v>2</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="7">
-        <v>5</v>
-      </c>
-      <c r="G35" s="7">
-        <v>2</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Subindo index.html login.html e cadastro.html (V1)
</commit_message>
<xml_diff>
--- a/Nike_Documentary/Backlog/BacklogNikeStepClub.xlsx
+++ b/Nike_Documentary/Backlog/BacklogNikeStepClub.xlsx
@@ -1070,6 +1070,9 @@
                 <c:pt idx="2">
                   <c:v>168</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>131</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1085,8 +1088,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="290317096"/>
-        <c:axId val="290314352"/>
+        <c:axId val="258097264"/>
+        <c:axId val="258805232"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -1202,7 +1205,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Planilha1!$N$1</c15:sqref>
@@ -1243,7 +1246,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Planilha1!$L$2:$L$6</c15:sqref>
@@ -1272,7 +1275,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Planilha1!$N$2:$N$6</c15:sqref>
@@ -1309,7 +1312,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Planilha1!$O$1</c15:sqref>
@@ -1350,7 +1353,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Planilha1!$L$2:$L$6</c15:sqref>
@@ -1379,7 +1382,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Planilha1!$O$2:$O$6</c15:sqref>
@@ -1390,13 +1393,16 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="5"/>
                       <c:pt idx="0">
-                        <c:v>114</c:v>
+                        <c:v>151</c:v>
                       </c:pt>
                       <c:pt idx="1">
                         <c:v>51</c:v>
                       </c:pt>
                       <c:pt idx="2">
                         <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>37</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1408,7 +1414,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="290317096"/>
+        <c:axId val="258097264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,7 +1457,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290314352"/>
+        <c:crossAx val="258805232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1459,7 +1465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290314352"/>
+        <c:axId val="258805232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1510,7 +1516,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290317096"/>
+        <c:crossAx val="258097264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2506,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2610,7 +2616,7 @@
       </c>
       <c r="O2" s="12">
         <f>SUM(O3,O4,O5,O6)</f>
-        <v>114</v>
+        <v>151</v>
       </c>
       <c r="P2" s="23">
         <v>282</v>
@@ -2766,12 +2772,17 @@
       <c r="N5" s="17">
         <v>84</v>
       </c>
-      <c r="O5" s="17"/>
+      <c r="O5" s="17">
+        <v>37</v>
+      </c>
       <c r="P5" s="16">
         <f>P4-N5</f>
         <v>81</v>
       </c>
-      <c r="Q5" s="22"/>
+      <c r="Q5" s="22">
+        <f>Q4-O5</f>
+        <v>131</v>
+      </c>
       <c r="R5" s="22"/>
     </row>
     <row r="6" spans="1:18">

</xml_diff>